<commit_message>
Cambios en las combinaciones únicas aclaración en el video de la reunion
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/Modelo De Dominio Enriquecido Residentes.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/Modelo De Dominio Enriquecido Residentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{ABFC273F-1EC1-4D7E-8700-159149DAF5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABD7C4E9-C9E3-4A41-944C-5301E4A0C05F}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="13_ncr:1_{ABFC273F-1EC1-4D7E-8700-159149DAF5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8E375C8-E4CF-48DB-AFB0-AF7FF4698801}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{007C2ECE-7E90-4717-B1E7-3A143C146FF0}"/>
   </bookViews>
@@ -898,7 +898,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="109">
   <si>
     <t>Tipo Objeto Dominio</t>
   </si>
@@ -1188,21 +1188,9 @@
     <t>Representa la contraseña de acceso que tiene un residente para poder ingresar a la aplicación de reservas.</t>
   </si>
   <si>
-    <t xml:space="preserve">Identificacion de residente </t>
-  </si>
-  <si>
-    <t>No es posible tener más de un residente con el mismo numero de identificador.</t>
-  </si>
-  <si>
     <t>numeroID</t>
   </si>
   <si>
-    <t>No es posible tener más de un residente con el mismo numero de identificación, el mismo correo electrónico y el mismo número de contacto.</t>
-  </si>
-  <si>
-    <t>numeroContacto</t>
-  </si>
-  <si>
     <t>tipoInmueble</t>
   </si>
   <si>
@@ -1231,6 +1219,12 @@
   </si>
   <si>
     <t>No es posible tener más de un inmueble con la misma zona inmueble, el mismo tipo inmueble, el mismo numero de vivienda, con el mismo identificador.</t>
+  </si>
+  <si>
+    <t>No es posible tener más de un residente con el mismo nombre, apellido, tipo de documento y numero documento para el mismo inmueble.</t>
+  </si>
+  <si>
+    <t>numeroDocumento</t>
   </si>
 </sst>
 </file>
@@ -1355,7 +1349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1657,45 +1651,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1720,9 +1675,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1736,13 +1722,24 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1909,6 +1906,18 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1927,6 +1936,69 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1951,45 +2023,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1999,71 +2032,35 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2462,10 +2459,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="61"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2585,11 +2582,11 @@
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="63"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -2615,7 +2612,7 @@
       <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="60" t="str">
+      <c r="D3" s="64" t="str">
         <f>$B$1</f>
         <v>Residentes</v>
       </c>
@@ -2631,7 +2628,7 @@
         <f>Valores!$A$4</f>
         <v>Referenciado</v>
       </c>
-      <c r="D4" s="61"/>
+      <c r="D4" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2649,8 +2646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CD2E3E-2179-4007-8743-BED3F3BF1317}">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2681,73 +2678,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="81" t="str">
+      <c r="B2" s="71" t="str">
         <f>'Listado Objetos de Dominio'!A3</f>
         <v>Residente</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="82" t="str">
+      <c r="B3" s="72" t="str">
         <f>'Listado Objetos de Dominio'!B3</f>
         <v>Objeto de dominio que representa a un residente que vive dentro de un inmueble en un conjunto residencial</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="72"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -2819,7 +2816,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="105" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="24" t="s">
@@ -3006,7 +3003,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B9" s="24" t="s">
         <v>13</v>
@@ -3313,101 +3310,97 @@
     </row>
     <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="94"/>
-      <c r="C17" s="95"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="75"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="96" t="s">
+      <c r="A18" s="56" t="s">
         <v>51</v>
       </c>
       <c r="B18" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="97" t="s">
+      <c r="C18" s="57" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="98" t="s">
+    <row r="19" spans="1:19" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="92" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="99" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="101" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="88" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="99" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="102"/>
-      <c r="B21" s="103"/>
-      <c r="C21" s="99" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="106"/>
-      <c r="B22" s="107"/>
-      <c r="C22" s="100" t="s">
-        <v>69</v>
+      <c r="B19" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="103"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="107" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="103"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="104"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="106" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="86" t="s">
+      <c r="A24" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="70"/>
-      <c r="C24" s="70" t="s">
+      <c r="B24" s="77"/>
+      <c r="C24" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="70" t="s">
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="I24" s="70"/>
-      <c r="J24" s="70"/>
-      <c r="K24" s="70" t="s">
+      <c r="I24" s="77"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="L24" s="70"/>
-      <c r="M24" s="70"/>
-      <c r="N24" s="70"/>
-      <c r="O24" s="70"/>
-      <c r="P24" s="70" t="s">
+      <c r="L24" s="77"/>
+      <c r="M24" s="77"/>
+      <c r="N24" s="77"/>
+      <c r="O24" s="77"/>
+      <c r="P24" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="Q24" s="70"/>
-      <c r="R24" s="70" t="s">
+      <c r="Q24" s="77"/>
+      <c r="R24" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="S24" s="71"/>
+      <c r="S24" s="83"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="87"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
+      <c r="A25" s="78"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
       <c r="H25" s="35" t="s">
         <v>59</v>
       </c>
@@ -3420,12 +3413,12 @@
       <c r="K25" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="L25" s="72" t="s">
+      <c r="L25" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M25" s="72"/>
-      <c r="N25" s="72"/>
-      <c r="O25" s="72"/>
+      <c r="M25" s="79"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="79"/>
       <c r="P25" s="35" t="s">
         <v>61</v>
       </c>
@@ -3440,92 +3433,92 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="73" t="s">
+      <c r="A26" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="74"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
       <c r="H26" s="14"/>
       <c r="I26" s="12"/>
       <c r="J26" s="13"/>
       <c r="K26" s="12"/>
-      <c r="L26" s="75"/>
-      <c r="M26" s="75"/>
-      <c r="N26" s="75"/>
-      <c r="O26" s="75"/>
+      <c r="L26" s="86"/>
+      <c r="M26" s="86"/>
+      <c r="N26" s="86"/>
+      <c r="O26" s="86"/>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="37"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="77"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
       <c r="H27" s="40"/>
       <c r="I27" s="38"/>
       <c r="J27" s="39"/>
       <c r="K27" s="41"/>
-      <c r="L27" s="79"/>
-      <c r="M27" s="79"/>
-      <c r="N27" s="79"/>
-      <c r="O27" s="79"/>
+      <c r="L27" s="69"/>
+      <c r="M27" s="69"/>
+      <c r="N27" s="69"/>
+      <c r="O27" s="69"/>
       <c r="P27" s="29"/>
       <c r="Q27" s="42"/>
       <c r="R27" s="42"/>
       <c r="S27" s="43"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" s="62" t="s">
+      <c r="A28" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="63"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
       <c r="H28" s="45"/>
       <c r="I28" s="46"/>
       <c r="J28" s="44"/>
       <c r="K28" s="47"/>
-      <c r="L28" s="65"/>
-      <c r="M28" s="65"/>
-      <c r="N28" s="65"/>
-      <c r="O28" s="65"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="90"/>
+      <c r="O28" s="90"/>
       <c r="P28" s="30"/>
       <c r="Q28" s="48"/>
       <c r="R28" s="48"/>
       <c r="S28" s="49"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="68"/>
+      <c r="B29" s="92"/>
+      <c r="C29" s="93"/>
+      <c r="D29" s="93"/>
+      <c r="E29" s="93"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="93"/>
       <c r="H29" s="51"/>
       <c r="I29" s="52"/>
       <c r="J29" s="50"/>
       <c r="K29" s="51"/>
-      <c r="L29" s="69"/>
-      <c r="M29" s="69"/>
-      <c r="N29" s="69"/>
-      <c r="O29" s="69"/>
+      <c r="L29" s="94"/>
+      <c r="M29" s="94"/>
+      <c r="N29" s="94"/>
+      <c r="O29" s="94"/>
       <c r="P29" s="31"/>
       <c r="Q29" s="53"/>
       <c r="R29" s="53"/>
@@ -3533,6 +3526,17 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="L26:O26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="L27:O27"/>
@@ -3545,19 +3549,8 @@
     <mergeCell ref="H24:J24"/>
     <mergeCell ref="K24:O24"/>
     <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="L25:O25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{475DC609-B6D5-4D2D-A170-5000DA801120}"/>
@@ -3571,11 +3564,12 @@
     <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{B80B22E6-6928-44D7-BF33-2D2339A3EAD3}"/>
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{2CEFD9A1-7256-4CC0-A14B-05D2869A5C81}"/>
     <hyperlink ref="A28:B28" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{35AD5D22-1DAF-4594-AD05-7CB9953F9873}"/>
-    <hyperlink ref="C19" location="Residente!A5" display="identificador" xr:uid="{44C56CF5-7141-4A21-B9BC-308CD3AA36CE}"/>
+    <hyperlink ref="C22" location="Residente!A9" display="numeroDocumento" xr:uid="{44C56CF5-7141-4A21-B9BC-308CD3AA36CE}"/>
     <hyperlink ref="I13" r:id="rId1" xr:uid="{DB94A35C-D1D9-4791-A75D-DEEACCA61A6F}"/>
-    <hyperlink ref="C20" location="Residente!A9" display="numeroID" xr:uid="{95281040-7DB2-4E3A-8C93-8D6AA71D6775}"/>
-    <hyperlink ref="C22" location="Residente!A13" display="correo" xr:uid="{B15B23D6-B740-4D59-9192-BEB377392DC9}"/>
-    <hyperlink ref="C21" location="Residente!A11" display="numeroContacto" xr:uid="{3F300411-4BD6-4CDE-B8C8-7ADAB2309295}"/>
+    <hyperlink ref="A5" location="Residente!A12" display="identificador" xr:uid="{A920818D-F9BB-43C7-8C7F-E02D95D9364D}"/>
+    <hyperlink ref="C19" location="Residente!A6" display="nombre" xr:uid="{1CBC68C4-BE94-4F2E-83D7-6456A248648E}"/>
+    <hyperlink ref="C20" location="Residente!A7" display="apellido" xr:uid="{14A0404A-8C91-4446-8FC5-A389C06298D8}"/>
+    <hyperlink ref="C21" location="Residente!A8" display="tipoDocumento" xr:uid="{54E136A1-DFED-46E9-8B2D-B46752A571BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>
@@ -3599,7 +3593,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3630,73 +3624,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="81" t="str">
+      <c r="B2" s="71" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Inmueble</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="82" t="str">
+      <c r="B3" s="72" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v xml:space="preserve">Objeto de dominio que representa el inmueble donde vive el residente del conjunto residencial. </v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="72"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -3814,7 +3808,7 @@
     </row>
     <row r="6" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>8</v>
@@ -3830,7 +3824,7 @@
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
       <c r="I6" s="25" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J6" s="24"/>
       <c r="K6" s="26"/>
@@ -3850,7 +3844,7 @@
         <v>42</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="R6" s="28"/>
       <c r="S6" s="29"/>
@@ -3859,10 +3853,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
@@ -3889,7 +3883,7 @@
         <v>42</v>
       </c>
       <c r="Q7" s="25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="R7" s="28"/>
       <c r="S7" s="29"/>
@@ -3898,10 +3892,10 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -3918,7 +3912,7 @@
       <c r="O8" s="24"/>
       <c r="P8" s="24"/>
       <c r="Q8" s="25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="R8" s="28"/>
       <c r="S8" s="29"/>
@@ -3927,11 +3921,11 @@
     </row>
     <row r="9" spans="1:21" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="85"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
@@ -3945,79 +3939,79 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="90" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" s="88" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="105" t="s">
+      <c r="A12" s="98" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="80" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="59" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="104"/>
-      <c r="B13" s="103"/>
-      <c r="C13" s="105" t="s">
-        <v>101</v>
+      <c r="A13" s="99"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="59" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="104"/>
-      <c r="B14" s="103"/>
-      <c r="C14" s="105" t="s">
-        <v>102</v>
+      <c r="A14" s="99"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="59" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="91"/>
-      <c r="B15" s="89"/>
+      <c r="A15" s="100"/>
+      <c r="B15" s="101"/>
       <c r="C15" s="55" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="86" t="s">
+      <c r="A17" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70" t="s">
+      <c r="B17" s="77"/>
+      <c r="C17" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70" t="s">
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="70" t="s">
+      <c r="I17" s="77"/>
+      <c r="J17" s="77"/>
+      <c r="K17" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="L17" s="70"/>
-      <c r="M17" s="70"/>
-      <c r="N17" s="70"/>
-      <c r="O17" s="70"/>
-      <c r="P17" s="70" t="s">
+      <c r="L17" s="77"/>
+      <c r="M17" s="77"/>
+      <c r="N17" s="77"/>
+      <c r="O17" s="77"/>
+      <c r="P17" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="Q17" s="70"/>
-      <c r="R17" s="70" t="s">
+      <c r="Q17" s="77"/>
+      <c r="R17" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="S17" s="71"/>
+      <c r="S17" s="83"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="87"/>
-      <c r="B18" s="72"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
       <c r="H18" s="35" t="s">
         <v>59</v>
       </c>
@@ -4030,12 +4024,12 @@
       <c r="K18" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="72" t="s">
+      <c r="L18" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M18" s="72"/>
-      <c r="N18" s="72"/>
-      <c r="O18" s="72"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="79"/>
       <c r="P18" s="35" t="s">
         <v>61</v>
       </c>
@@ -4050,92 +4044,92 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
       <c r="H19" s="14"/>
       <c r="I19" s="12"/>
       <c r="J19" s="13"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="75"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="86"/>
+      <c r="N19" s="86"/>
+      <c r="O19" s="86"/>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
       <c r="R19" s="14"/>
       <c r="S19" s="37"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="77"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
       <c r="H20" s="40"/>
       <c r="I20" s="38"/>
       <c r="J20" s="39"/>
       <c r="K20" s="41"/>
-      <c r="L20" s="79"/>
-      <c r="M20" s="79"/>
-      <c r="N20" s="79"/>
-      <c r="O20" s="79"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="69"/>
       <c r="P20" s="29"/>
       <c r="Q20" s="42"/>
       <c r="R20" s="42"/>
       <c r="S20" s="43"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="62" t="s">
+      <c r="A21" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="89"/>
       <c r="H21" s="45"/>
       <c r="I21" s="46"/>
       <c r="J21" s="44"/>
       <c r="K21" s="47"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="65"/>
+      <c r="L21" s="90"/>
+      <c r="M21" s="90"/>
+      <c r="N21" s="90"/>
+      <c r="O21" s="90"/>
       <c r="P21" s="30"/>
       <c r="Q21" s="48"/>
       <c r="R21" s="48"/>
       <c r="S21" s="49"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="67"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
       <c r="H22" s="51"/>
       <c r="I22" s="52"/>
       <c r="J22" s="50"/>
       <c r="K22" s="51"/>
-      <c r="L22" s="69"/>
-      <c r="M22" s="69"/>
-      <c r="N22" s="69"/>
-      <c r="O22" s="69"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="94"/>
+      <c r="O22" s="94"/>
       <c r="P22" s="31"/>
       <c r="Q22" s="53"/>
       <c r="R22" s="53"/>
@@ -4143,12 +4137,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
     <mergeCell ref="P17:Q17"/>
     <mergeCell ref="R17:S17"/>
     <mergeCell ref="A20:B20"/>
@@ -4162,12 +4156,12 @@
     <mergeCell ref="C17:G18"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="K17:O17"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="L22:O22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{ABE5976C-7405-4C29-983F-966BEFED6A8B}"/>

</xml_diff>

<commit_message>
Creación de las relaciones importantes entre contextos en el modelo de dominio anemico
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/Modelo De Dominio Enriquecido Residentes.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Modelos de Dominio Enriquecidos/Modelo De Dominio Enriquecido Residentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Nueva Version Victus\Modelos de Dominio Enriquecidos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\Modelos de Dominio Enriquecidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4E4593-E791-4455-9E80-D1D50C723C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B9D03A-DE01-40F9-B98E-CDD20DFEBEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="3" activeTab="4" xr2:uid="{007C2ECE-7E90-4717-B1E7-3A143C146FF0}"/>
+    <workbookView minimized="1" xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="8880" firstSheet="4" activeTab="4" xr2:uid="{007C2ECE-7E90-4717-B1E7-3A143C146FF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
@@ -1727,86 +1727,86 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2198,19 +2198,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="57"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -2234,52 +2234,52 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -2300,7 +2300,7 @@
       <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2315,16 +2315,16 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="7"/>
+    <col min="1" max="1" width="21.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>16</v>
       </c>
@@ -2334,7 +2334,7 @@
       <c r="C1" s="58"/>
       <c r="D1" s="59"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>Residentes</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>72</v>
       </c>
@@ -2396,103 +2396,103 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="79.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="7"/>
+    <col min="17" max="17" width="94.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="71" t="str">
+      <c r="B2" s="78" t="str">
         <f>'Listado Objetos de Dominio'!A3</f>
         <v>Residente</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="72" t="str">
+      <c r="B3" s="79" t="str">
         <f>'Listado Objetos de Dominio'!B3</f>
         <v>Objeto de dominio que representa a un residente que vive dentro de un inmueble en un conjunto residencial</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="79"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="52" t="s">
         <v>39</v>
       </c>
@@ -2606,7 +2606,7 @@
       <c r="T5" s="29"/>
       <c r="U5" s="30"/>
     </row>
-    <row r="6" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>43</v>
       </c>
@@ -2653,7 +2653,7 @@
       <c r="T6" s="29"/>
       <c r="U6" s="30"/>
     </row>
-    <row r="7" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>67</v>
       </c>
@@ -2700,7 +2700,7 @@
       <c r="T7" s="29"/>
       <c r="U7" s="30"/>
     </row>
-    <row r="8" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>75</v>
       </c>
@@ -2747,7 +2747,7 @@
       <c r="T8" s="29"/>
       <c r="U8" s="30"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>86</v>
       </c>
@@ -2788,7 +2788,7 @@
       <c r="T9" s="29"/>
       <c r="U9" s="30"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>68</v>
       </c>
@@ -2829,7 +2829,7 @@
       <c r="T10" s="29"/>
       <c r="U10" s="30"/>
     </row>
-    <row r="11" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>87</v>
       </c>
@@ -2872,7 +2872,7 @@
       <c r="T11" s="29"/>
       <c r="U11" s="30"/>
     </row>
-    <row r="12" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>102</v>
       </c>
@@ -2919,7 +2919,7 @@
       <c r="T12" s="29"/>
       <c r="U12" s="30"/>
     </row>
-    <row r="13" spans="1:21" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>76</v>
       </c>
@@ -2966,7 +2966,7 @@
       <c r="T13" s="29"/>
       <c r="U13" s="30"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>69</v>
       </c>
@@ -3007,24 +3007,24 @@
       <c r="T14" s="29"/>
       <c r="U14" s="30"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="E16" s="64" t="s">
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="E16" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="I16" s="64" t="s">
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="I16" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="64"/>
-      <c r="K16" s="64"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="31" t="s">
         <v>48</v>
       </c>
@@ -3053,114 +3053,114 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="65" t="s">
+    <row r="18" spans="1:19" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="84" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="63" t="s">
+      <c r="E18" s="84" t="s">
         <v>103</v>
       </c>
-      <c r="F18" s="63" t="s">
+      <c r="F18" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="G18" s="62" t="s">
+      <c r="G18" s="88" t="s">
         <v>87</v>
       </c>
       <c r="H18" s="54"/>
-      <c r="I18" s="65" t="s">
+      <c r="I18" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="J18" s="63" t="s">
+      <c r="J18" s="84" t="s">
         <v>101</v>
       </c>
-      <c r="K18" s="62" t="s">
+      <c r="K18" s="88" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="65"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="62"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="62"/>
+    <row r="19" spans="1:19" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="83"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="88"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="88"/>
       <c r="H19" s="54"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="62"/>
-    </row>
-    <row r="20" spans="1:19" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="65"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="62" t="s">
+      <c r="I19" s="83"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="88"/>
+    </row>
+    <row r="20" spans="1:19" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="83"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="62"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="62"/>
-    </row>
-    <row r="21" spans="1:19" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="65"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="62"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="62"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="63"/>
-      <c r="K21" s="62"/>
-    </row>
-    <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="73" t="s">
+      <c r="E20" s="84"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="88"/>
+      <c r="I20" s="83"/>
+      <c r="J20" s="84"/>
+      <c r="K20" s="88"/>
+    </row>
+    <row r="21" spans="1:19" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="83"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="88"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="88"/>
+      <c r="I21" s="83"/>
+      <c r="J21" s="84"/>
+      <c r="K21" s="88"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74" t="s">
+      <c r="B23" s="70"/>
+      <c r="C23" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74" t="s">
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="74" t="s">
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="L23" s="74"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="74"/>
-      <c r="O23" s="74"/>
-      <c r="P23" s="74" t="s">
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
+      <c r="N23" s="70"/>
+      <c r="O23" s="70"/>
+      <c r="P23" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="Q23" s="74"/>
-      <c r="R23" s="74" t="s">
+      <c r="Q23" s="70"/>
+      <c r="R23" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="S23" s="77"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="75"/>
-      <c r="B24" s="76"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
+      <c r="S23" s="71"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="82"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
       <c r="H24" s="32" t="s">
         <v>56</v>
       </c>
@@ -3173,12 +3173,12 @@
       <c r="K24" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="L24" s="76" t="s">
+      <c r="L24" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="M24" s="76"/>
-      <c r="N24" s="76"/>
-      <c r="O24" s="76"/>
+      <c r="M24" s="72"/>
+      <c r="N24" s="72"/>
+      <c r="O24" s="72"/>
       <c r="P24" s="32" t="s">
         <v>58</v>
       </c>
@@ -3192,93 +3192,93 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="78" t="s">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="80"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
       <c r="H25" s="13"/>
       <c r="I25" s="11"/>
       <c r="J25" s="12"/>
       <c r="K25" s="11"/>
-      <c r="L25" s="80"/>
-      <c r="M25" s="80"/>
-      <c r="N25" s="80"/>
-      <c r="O25" s="80"/>
+      <c r="L25" s="75"/>
+      <c r="M25" s="75"/>
+      <c r="N25" s="75"/>
+      <c r="O25" s="75"/>
       <c r="P25" s="13"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
       <c r="S25" s="34"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="66" t="s">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
       <c r="H26" s="37"/>
       <c r="I26" s="35"/>
       <c r="J26" s="36"/>
       <c r="K26" s="38"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="69"/>
-      <c r="N26" s="69"/>
-      <c r="O26" s="69"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="76"/>
+      <c r="O26" s="76"/>
       <c r="P26" s="28"/>
       <c r="Q26" s="39"/>
       <c r="R26" s="39"/>
       <c r="S26" s="40"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="81" t="s">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="82"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="83"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
       <c r="H27" s="42"/>
       <c r="I27" s="43"/>
       <c r="J27" s="41"/>
       <c r="K27" s="44"/>
-      <c r="L27" s="84"/>
-      <c r="M27" s="84"/>
-      <c r="N27" s="84"/>
-      <c r="O27" s="84"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
       <c r="P27" s="29"/>
       <c r="Q27" s="45"/>
       <c r="R27" s="45"/>
       <c r="S27" s="46"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="85" t="s">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="86"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
       <c r="H28" s="48"/>
       <c r="I28" s="49"/>
       <c r="J28" s="47"/>
       <c r="K28" s="48"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="88"/>
-      <c r="N28" s="88"/>
-      <c r="O28" s="88"/>
+      <c r="L28" s="69"/>
+      <c r="M28" s="69"/>
+      <c r="N28" s="69"/>
+      <c r="O28" s="69"/>
       <c r="P28" s="30"/>
       <c r="Q28" s="50"/>
       <c r="R28" s="50"/>
@@ -3286,17 +3286,14 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="L27:O27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="G18:G21"/>
     <mergeCell ref="L26:O26"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:Q2"/>
@@ -3313,14 +3310,17 @@
     <mergeCell ref="E18:E21"/>
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="I18:I21"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="L28:O28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{475DC609-B6D5-4D2D-A170-5000DA801120}"/>
@@ -3363,106 +3363,106 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:Q3"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="79.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="7"/>
+    <col min="17" max="17" width="94.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="71" t="str">
+      <c r="B2" s="78" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Inmueble</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="72" t="str">
+      <c r="B3" s="79" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v xml:space="preserve">Objeto de dominio que representa el inmueble donde vive el residente del conjunto residencial. </v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="79"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>39</v>
       </c>
@@ -3576,7 +3576,7 @@
       <c r="T5" s="29"/>
       <c r="U5" s="30"/>
     </row>
-    <row r="6" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>80</v>
       </c>
@@ -3621,7 +3621,7 @@
       <c r="T6" s="29"/>
       <c r="U6" s="30"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>81</v>
       </c>
@@ -3664,7 +3664,7 @@
       <c r="T7" s="29"/>
       <c r="U7" s="30"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>82</v>
       </c>
@@ -3693,15 +3693,15 @@
       <c r="T8" s="29"/>
       <c r="U8" s="30"/>
     </row>
-    <row r="9" spans="1:21" ht="23.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="64" t="s">
+    <row r="9" spans="1:21" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>48</v>
       </c>
@@ -3712,78 +3712,78 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="63" t="s">
+    <row r="12" spans="1:21" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="88" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="62"/>
-    </row>
-    <row r="14" spans="1:21" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="63"/>
-      <c r="B14" s="63"/>
+    <row r="13" spans="1:21" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="84"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="88"/>
+    </row>
+    <row r="14" spans="1:21" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="84"/>
+      <c r="B14" s="84"/>
       <c r="C14" s="53" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="63"/>
-      <c r="B15" s="63"/>
+    <row r="15" spans="1:21" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="84"/>
+      <c r="B15" s="84"/>
       <c r="C15" s="53" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="73" t="s">
+    <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74" t="s">
+      <c r="B17" s="70"/>
+      <c r="C17" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74" t="s">
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74" t="s">
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="L17" s="74"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74"/>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74" t="s">
+      <c r="L17" s="70"/>
+      <c r="M17" s="70"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="70"/>
+      <c r="P17" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74" t="s">
+      <c r="Q17" s="70"/>
+      <c r="R17" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="S17" s="77"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
+      <c r="S17" s="71"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="82"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
       <c r="H18" s="32" t="s">
         <v>56</v>
       </c>
@@ -3796,12 +3796,12 @@
       <c r="K18" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="76" t="s">
+      <c r="L18" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="M18" s="76"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="76"/>
+      <c r="M18" s="72"/>
+      <c r="N18" s="72"/>
+      <c r="O18" s="72"/>
       <c r="P18" s="32" t="s">
         <v>58</v>
       </c>
@@ -3815,93 +3815,93 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="78" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="80"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
       <c r="H19" s="13"/>
       <c r="I19" s="11"/>
       <c r="J19" s="12"/>
       <c r="K19" s="11"/>
-      <c r="L19" s="80"/>
-      <c r="M19" s="80"/>
-      <c r="N19" s="80"/>
-      <c r="O19" s="80"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="75"/>
+      <c r="N19" s="75"/>
+      <c r="O19" s="75"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
       <c r="R19" s="13"/>
       <c r="S19" s="34"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="66" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
       <c r="H20" s="37"/>
       <c r="I20" s="35"/>
       <c r="J20" s="36"/>
       <c r="K20" s="38"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
+      <c r="L20" s="76"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="76"/>
+      <c r="O20" s="76"/>
       <c r="P20" s="28"/>
       <c r="Q20" s="39"/>
       <c r="R20" s="39"/>
       <c r="S20" s="40"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="81" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="82"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="42"/>
       <c r="I21" s="43"/>
       <c r="J21" s="41"/>
       <c r="K21" s="44"/>
-      <c r="L21" s="84"/>
-      <c r="M21" s="84"/>
-      <c r="N21" s="84"/>
-      <c r="O21" s="84"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="65"/>
+      <c r="N21" s="65"/>
+      <c r="O21" s="65"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="45"/>
       <c r="R21" s="45"/>
       <c r="S21" s="46"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="85" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="86"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
       <c r="H22" s="48"/>
       <c r="I22" s="49"/>
       <c r="J22" s="47"/>
       <c r="K22" s="48"/>
-      <c r="L22" s="88"/>
-      <c r="M22" s="88"/>
-      <c r="N22" s="88"/>
-      <c r="O22" s="88"/>
+      <c r="L22" s="69"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="69"/>
+      <c r="O22" s="69"/>
       <c r="P22" s="30"/>
       <c r="Q22" s="50"/>
       <c r="R22" s="50"/>
@@ -3909,13 +3909,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="L22:O22"/>
     <mergeCell ref="P17:Q17"/>
     <mergeCell ref="R17:S17"/>
     <mergeCell ref="A20:B20"/>
@@ -3929,12 +3928,13 @@
     <mergeCell ref="C17:G18"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="K17:O17"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{4C6EA31D-5DD1-42F9-A469-ED5E8CAE0643}"/>

</xml_diff>